<commit_message>
test data fetching technique based on test case id.
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\data_driven_framework\DataDrivenFramework1\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAC2667-6B64-4EC2-BA7C-0A7D2DA5ECF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394D9CC4-28B8-4928-AA1A-53FA9DAD6AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
   <si>
     <t>TestDataHeader1</t>
   </si>
@@ -205,124 +205,46 @@
     <t>TC10_TestDataCell58</t>
   </si>
   <si>
-    <t>TC1_TestDataCell11</t>
-  </si>
-  <si>
-    <t>TC1_TestDataCell12</t>
-  </si>
-  <si>
-    <t>TC1_TestDataCell13</t>
-  </si>
-  <si>
-    <t>TC1_TestDataCell14</t>
-  </si>
-  <si>
-    <t>TC1_TestDataCell15</t>
-  </si>
-  <si>
-    <t>TC1_TestDataCell16</t>
-  </si>
-  <si>
-    <t>TC1_TestDataCell17</t>
-  </si>
-  <si>
-    <t>TC1_TestDataCell18</t>
-  </si>
-  <si>
-    <t>TC2_TestDataCell21</t>
-  </si>
-  <si>
-    <t>TC2_TestDataCell22</t>
-  </si>
-  <si>
-    <t>TC2_TestDataCell23</t>
-  </si>
-  <si>
-    <t>TC2_TestDataCell24</t>
-  </si>
-  <si>
-    <t>TC2_TestDataCell25</t>
-  </si>
-  <si>
-    <t>TC2_TestDataCell26</t>
-  </si>
-  <si>
-    <t>TC2_TestDataCell27</t>
-  </si>
-  <si>
-    <t>TC2_TestDataCell28</t>
-  </si>
-  <si>
-    <t>TC3_TestDataCell31</t>
-  </si>
-  <si>
-    <t>TC3_TestDataCell32</t>
-  </si>
-  <si>
-    <t>TC3_TestDataCell33</t>
-  </si>
-  <si>
-    <t>TC3_TestDataCell34</t>
-  </si>
-  <si>
-    <t>TC3_TestDataCell35</t>
-  </si>
-  <si>
-    <t>TC3_TestDataCell36</t>
-  </si>
-  <si>
-    <t>TC3_TestDataCell37</t>
-  </si>
-  <si>
-    <t>TC3_TestDataCell38</t>
-  </si>
-  <si>
-    <t>TC4_TestDataCell41</t>
-  </si>
-  <si>
-    <t>TC4_TestDataCell42</t>
-  </si>
-  <si>
-    <t>TC4_TestDataCell43</t>
-  </si>
-  <si>
-    <t>TC4_TestDataCell44</t>
-  </si>
-  <si>
-    <t>TC4_TestDataCell45</t>
-  </si>
-  <si>
-    <t>TC4_TestDataCell46</t>
-  </si>
-  <si>
-    <t>TC4_TestDataCell47</t>
-  </si>
-  <si>
-    <t>TC4_TestDataCell48</t>
-  </si>
-  <si>
-    <t>TC5_TestDataCell51</t>
-  </si>
-  <si>
-    <t>TC5_TestDataCell52</t>
-  </si>
-  <si>
-    <t>TC5_TestDataCell53</t>
-  </si>
-  <si>
-    <t>TC5_TestDataCell54</t>
-  </si>
-  <si>
-    <t>TC5_TestDataCell55</t>
-  </si>
-  <si>
-    <t>TC5_TestDataCell56</t>
-  </si>
-  <si>
-    <t>TC5_TestDataCell57</t>
-  </si>
-  <si>
-    <t>TC5_TestDataCell58</t>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sachin </t>
+  </si>
+  <si>
+    <t>Ramesh</t>
+  </si>
+  <si>
+    <t>Vijay</t>
+  </si>
+  <si>
+    <t>Akash</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Gupta</t>
+  </si>
+  <si>
+    <t>Patil</t>
+  </si>
+  <si>
+    <t>Deshpande</t>
+  </si>
+  <si>
+    <t>Bhosle</t>
   </si>
 </sst>
 </file>
@@ -677,10 +599,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="17.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C5F0B0-7C10-445C-9E41-012FAA290AFE}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,200 +764,6 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C5F0B0-7C10-445C-9E41-012FAA290AFE}">
-  <dimension ref="A1:I6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="17.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">

</xml_diff>